<commit_message>
Fix download url of service record
</commit_message>
<xml_diff>
--- a/public/SERVICE_RECORD.xlsx
+++ b/public/SERVICE_RECORD.xlsx
@@ -611,7 +611,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
@@ -731,29 +731,28 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="2" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="2" borderId="1" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -789,29 +788,38 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="2" borderId="1" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="2" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1125,8 +1133,8 @@
   </sheetPr>
   <dimension ref="A1:J72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1144,72 +1152,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="67"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
     </row>
     <row r="3" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A3" s="72" t="s">
+      <c r="A3" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="72"/>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="68" t="s">
+      <c r="A4" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="68"/>
-      <c r="C4" s="68"/>
-      <c r="D4" s="68"/>
-      <c r="E4" s="68"/>
-      <c r="F4" s="68"/>
-      <c r="G4" s="68"/>
-      <c r="H4" s="68"/>
-      <c r="I4" s="68"/>
-      <c r="J4" s="68"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="53"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="68"/>
-      <c r="B5" s="68"/>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="68"/>
-      <c r="H5" s="68"/>
-      <c r="I5" s="68"/>
-      <c r="J5" s="68"/>
+      <c r="A5" s="53"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="53"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -1221,17 +1229,17 @@
       <c r="C6" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="71" t="s">
+      <c r="D6" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="71"/>
-      <c r="F6" s="67" t="s">
+      <c r="E6" s="48"/>
+      <c r="F6" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="67"/>
-      <c r="H6" s="67"/>
-      <c r="I6" s="67"/>
-      <c r="J6" s="67"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="49"/>
+      <c r="I6" s="49"/>
+      <c r="J6" s="49"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
@@ -1241,15 +1249,15 @@
       <c r="C7" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="69" t="s">
+      <c r="D7" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="69"/>
-      <c r="F7" s="68"/>
-      <c r="G7" s="68"/>
-      <c r="H7" s="68"/>
-      <c r="I7" s="68"/>
-      <c r="J7" s="68"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
@@ -1264,22 +1272,22 @@
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="67" t="s">
+      <c r="A9" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="67"/>
-      <c r="C9" s="73" t="s">
+      <c r="B9" s="49"/>
+      <c r="C9" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="74" t="s">
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="74"/>
-      <c r="H9" s="74"/>
-      <c r="I9" s="74"/>
-      <c r="J9" s="74"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="52"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
@@ -1287,11 +1295,11 @@
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="74"/>
-      <c r="G10" s="74"/>
-      <c r="H10" s="74"/>
-      <c r="I10" s="74"/>
-      <c r="J10" s="74"/>
+      <c r="F10" s="52"/>
+      <c r="G10" s="52"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="52"/>
+      <c r="J10" s="52"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
@@ -1299,22 +1307,22 @@
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="74"/>
-      <c r="G11" s="74"/>
-      <c r="H11" s="74"/>
-      <c r="I11" s="74"/>
-      <c r="J11" s="74"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="52"/>
+      <c r="H11" s="52"/>
+      <c r="I11" s="52"/>
+      <c r="J11" s="52"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="1"/>
-      <c r="C12" s="70" t="s">
+      <c r="C12" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="70"/>
-      <c r="E12" s="70"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -1334,42 +1342,42 @@
       <c r="J13" s="1"/>
     </row>
     <row r="14" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="58" t="s">
+      <c r="A14" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="59"/>
-      <c r="C14" s="59"/>
-      <c r="D14" s="59"/>
-      <c r="E14" s="59"/>
-      <c r="F14" s="59"/>
-      <c r="G14" s="59"/>
-      <c r="H14" s="59"/>
-      <c r="I14" s="59"/>
-      <c r="J14" s="59"/>
+      <c r="B14" s="58"/>
+      <c r="C14" s="58"/>
+      <c r="D14" s="58"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="58"/>
+      <c r="G14" s="58"/>
+      <c r="H14" s="58"/>
+      <c r="I14" s="58"/>
+      <c r="J14" s="58"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="59"/>
-      <c r="B15" s="59"/>
-      <c r="C15" s="59"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="59"/>
-      <c r="H15" s="59"/>
-      <c r="I15" s="59"/>
-      <c r="J15" s="59"/>
+      <c r="A15" s="58"/>
+      <c r="B15" s="58"/>
+      <c r="C15" s="58"/>
+      <c r="D15" s="58"/>
+      <c r="E15" s="58"/>
+      <c r="F15" s="58"/>
+      <c r="G15" s="58"/>
+      <c r="H15" s="58"/>
+      <c r="I15" s="58"/>
+      <c r="J15" s="58"/>
     </row>
     <row r="16" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="60"/>
-      <c r="B16" s="60"/>
-      <c r="C16" s="60"/>
-      <c r="D16" s="60"/>
-      <c r="E16" s="60"/>
-      <c r="F16" s="60"/>
-      <c r="G16" s="60"/>
-      <c r="H16" s="60"/>
-      <c r="I16" s="60"/>
-      <c r="J16" s="60"/>
+      <c r="A16" s="59"/>
+      <c r="B16" s="59"/>
+      <c r="C16" s="59"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="59"/>
+      <c r="F16" s="59"/>
+      <c r="G16" s="59"/>
+      <c r="H16" s="59"/>
+      <c r="I16" s="59"/>
+      <c r="J16" s="59"/>
     </row>
     <row r="17" spans="1:10" ht="6" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A17" s="7"/>
@@ -1380,10 +1388,10 @@
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="8"/>
-      <c r="I17" s="61" t="s">
+      <c r="I17" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="J17" s="62"/>
+      <c r="J17" s="61"/>
     </row>
     <row r="18" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
@@ -1400,8 +1408,8 @@
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="12"/>
-      <c r="I18" s="63"/>
-      <c r="J18" s="64"/>
+      <c r="I18" s="62"/>
+      <c r="J18" s="63"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
@@ -1424,8 +1432,8 @@
       <c r="H19" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="I19" s="63"/>
-      <c r="J19" s="64"/>
+      <c r="I19" s="62"/>
+      <c r="J19" s="63"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
@@ -1450,8 +1458,8 @@
         <v>25</v>
       </c>
       <c r="H20" s="16"/>
-      <c r="I20" s="63"/>
-      <c r="J20" s="64"/>
+      <c r="I20" s="62"/>
+      <c r="J20" s="63"/>
     </row>
     <row r="21" spans="1:10" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="18"/>
@@ -1462,20 +1470,20 @@
       <c r="F21" s="18"/>
       <c r="G21" s="18"/>
       <c r="H21" s="18"/>
-      <c r="I21" s="65"/>
-      <c r="J21" s="66"/>
+      <c r="I21" s="64"/>
+      <c r="J21" s="65"/>
     </row>
     <row r="22" spans="1:10" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A22" s="42"/>
       <c r="B22" s="42"/>
-      <c r="C22" s="43"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="47"/>
+      <c r="C22" s="75"/>
+      <c r="D22" s="74"/>
+      <c r="E22" s="76"/>
       <c r="F22" s="31"/>
-      <c r="G22" s="30"/>
+      <c r="G22" s="74"/>
       <c r="H22" s="31"/>
-      <c r="I22" s="56"/>
-      <c r="J22" s="57"/>
+      <c r="I22" s="55"/>
+      <c r="J22" s="56"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="42"/>
@@ -1486,8 +1494,8 @@
       <c r="F23" s="31"/>
       <c r="G23" s="30"/>
       <c r="H23" s="31"/>
-      <c r="I23" s="56"/>
-      <c r="J23" s="57"/>
+      <c r="I23" s="55"/>
+      <c r="J23" s="56"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="42"/>
@@ -1498,8 +1506,8 @@
       <c r="F24" s="31"/>
       <c r="G24" s="30"/>
       <c r="H24" s="31"/>
-      <c r="I24" s="56"/>
-      <c r="J24" s="57"/>
+      <c r="I24" s="55"/>
+      <c r="J24" s="56"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="42"/>
@@ -1510,8 +1518,8 @@
       <c r="F25" s="31"/>
       <c r="G25" s="30"/>
       <c r="H25" s="31"/>
-      <c r="I25" s="56"/>
-      <c r="J25" s="57"/>
+      <c r="I25" s="55"/>
+      <c r="J25" s="56"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="42"/>
@@ -1522,8 +1530,8 @@
       <c r="F26" s="31"/>
       <c r="G26" s="33"/>
       <c r="H26" s="31"/>
-      <c r="I26" s="56"/>
-      <c r="J26" s="57"/>
+      <c r="I26" s="55"/>
+      <c r="J26" s="56"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="42"/>
@@ -1534,8 +1542,8 @@
       <c r="F27" s="31"/>
       <c r="G27" s="33"/>
       <c r="H27" s="31"/>
-      <c r="I27" s="56"/>
-      <c r="J27" s="57"/>
+      <c r="I27" s="55"/>
+      <c r="J27" s="56"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="42"/>
@@ -1546,8 +1554,8 @@
       <c r="F28" s="35"/>
       <c r="G28" s="33"/>
       <c r="H28" s="31"/>
-      <c r="I28" s="56"/>
-      <c r="J28" s="57"/>
+      <c r="I28" s="55"/>
+      <c r="J28" s="56"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="42"/>
@@ -1558,8 +1566,8 @@
       <c r="F29" s="35"/>
       <c r="G29" s="33"/>
       <c r="H29" s="31"/>
-      <c r="I29" s="56"/>
-      <c r="J29" s="57"/>
+      <c r="I29" s="55"/>
+      <c r="J29" s="56"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="42"/>
@@ -1570,8 +1578,8 @@
       <c r="F30" s="35"/>
       <c r="G30" s="33"/>
       <c r="H30" s="31"/>
-      <c r="I30" s="56"/>
-      <c r="J30" s="57"/>
+      <c r="I30" s="55"/>
+      <c r="J30" s="56"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="42"/>
@@ -1582,8 +1590,8 @@
       <c r="F31" s="35"/>
       <c r="G31" s="33"/>
       <c r="H31" s="31"/>
-      <c r="I31" s="56"/>
-      <c r="J31" s="57"/>
+      <c r="I31" s="55"/>
+      <c r="J31" s="56"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="42"/>
@@ -1594,8 +1602,8 @@
       <c r="F32" s="35"/>
       <c r="G32" s="33"/>
       <c r="H32" s="31"/>
-      <c r="I32" s="56"/>
-      <c r="J32" s="57"/>
+      <c r="I32" s="55"/>
+      <c r="J32" s="56"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="42"/>
@@ -1606,8 +1614,8 @@
       <c r="F33" s="35"/>
       <c r="G33" s="33"/>
       <c r="H33" s="31"/>
-      <c r="I33" s="56"/>
-      <c r="J33" s="57"/>
+      <c r="I33" s="55"/>
+      <c r="J33" s="56"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="42"/>
@@ -1618,8 +1626,8 @@
       <c r="F34" s="35"/>
       <c r="G34" s="33"/>
       <c r="H34" s="31"/>
-      <c r="I34" s="54"/>
-      <c r="J34" s="55"/>
+      <c r="I34" s="66"/>
+      <c r="J34" s="67"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="42"/>
@@ -1630,8 +1638,8 @@
       <c r="F35" s="35"/>
       <c r="G35" s="33"/>
       <c r="H35" s="31"/>
-      <c r="I35" s="54"/>
-      <c r="J35" s="55"/>
+      <c r="I35" s="66"/>
+      <c r="J35" s="67"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="42"/>
@@ -1642,8 +1650,8 @@
       <c r="F36" s="35"/>
       <c r="G36" s="33"/>
       <c r="H36" s="31"/>
-      <c r="I36" s="56"/>
-      <c r="J36" s="57"/>
+      <c r="I36" s="55"/>
+      <c r="J36" s="56"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="42"/>
@@ -1654,8 +1662,8 @@
       <c r="F37" s="35"/>
       <c r="G37" s="33"/>
       <c r="H37" s="31"/>
-      <c r="I37" s="56"/>
-      <c r="J37" s="57"/>
+      <c r="I37" s="55"/>
+      <c r="J37" s="56"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="42"/>
@@ -1666,8 +1674,8 @@
       <c r="F38" s="35"/>
       <c r="G38" s="33"/>
       <c r="H38" s="31"/>
-      <c r="I38" s="56"/>
-      <c r="J38" s="57"/>
+      <c r="I38" s="55"/>
+      <c r="J38" s="56"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="42"/>
@@ -1678,8 +1686,8 @@
       <c r="F39" s="35"/>
       <c r="G39" s="33"/>
       <c r="H39" s="31"/>
-      <c r="I39" s="56"/>
-      <c r="J39" s="57"/>
+      <c r="I39" s="55"/>
+      <c r="J39" s="56"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="28"/>
@@ -1690,8 +1698,8 @@
       <c r="F40" s="35"/>
       <c r="G40" s="33"/>
       <c r="H40" s="26"/>
-      <c r="I40" s="48"/>
-      <c r="J40" s="49"/>
+      <c r="I40" s="68"/>
+      <c r="J40" s="69"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="28"/>
@@ -1702,8 +1710,8 @@
       <c r="F41" s="39"/>
       <c r="G41" s="21"/>
       <c r="H41" s="26"/>
-      <c r="I41" s="48"/>
-      <c r="J41" s="49"/>
+      <c r="I41" s="68"/>
+      <c r="J41" s="69"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="28"/>
@@ -1714,8 +1722,8 @@
       <c r="F42" s="35"/>
       <c r="G42" s="33"/>
       <c r="H42" s="26"/>
-      <c r="I42" s="56"/>
-      <c r="J42" s="57"/>
+      <c r="I42" s="55"/>
+      <c r="J42" s="56"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="28"/>
@@ -1726,8 +1734,8 @@
       <c r="F43" s="35"/>
       <c r="G43" s="33"/>
       <c r="H43" s="26"/>
-      <c r="I43" s="54"/>
-      <c r="J43" s="55"/>
+      <c r="I43" s="66"/>
+      <c r="J43" s="67"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="28"/>
@@ -1738,8 +1746,8 @@
       <c r="F44" s="35"/>
       <c r="G44" s="33"/>
       <c r="H44" s="26"/>
-      <c r="I44" s="54"/>
-      <c r="J44" s="55"/>
+      <c r="I44" s="66"/>
+      <c r="J44" s="67"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="28"/>
@@ -1750,8 +1758,8 @@
       <c r="F45" s="35"/>
       <c r="G45" s="33"/>
       <c r="H45" s="26"/>
-      <c r="I45" s="52"/>
-      <c r="J45" s="53"/>
+      <c r="I45" s="70"/>
+      <c r="J45" s="71"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="28"/>
@@ -1762,8 +1770,8 @@
       <c r="F46" s="36"/>
       <c r="G46" s="21"/>
       <c r="H46" s="26"/>
-      <c r="I46" s="48"/>
-      <c r="J46" s="49"/>
+      <c r="I46" s="68"/>
+      <c r="J46" s="69"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="28"/>
@@ -1774,8 +1782,8 @@
       <c r="F47" s="35"/>
       <c r="G47" s="33"/>
       <c r="H47" s="26"/>
-      <c r="I47" s="56"/>
-      <c r="J47" s="57"/>
+      <c r="I47" s="55"/>
+      <c r="J47" s="56"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="28"/>
@@ -1786,8 +1794,8 @@
       <c r="F48" s="36"/>
       <c r="G48" s="21"/>
       <c r="H48" s="26"/>
-      <c r="I48" s="52"/>
-      <c r="J48" s="53"/>
+      <c r="I48" s="70"/>
+      <c r="J48" s="71"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="28"/>
@@ -1798,8 +1806,8 @@
       <c r="F49" s="36"/>
       <c r="G49" s="21"/>
       <c r="H49" s="26"/>
-      <c r="I49" s="48"/>
-      <c r="J49" s="49"/>
+      <c r="I49" s="68"/>
+      <c r="J49" s="69"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="28"/>
@@ -1810,8 +1818,8 @@
       <c r="F50" s="36"/>
       <c r="G50" s="21"/>
       <c r="H50" s="41"/>
-      <c r="I50" s="48"/>
-      <c r="J50" s="49"/>
+      <c r="I50" s="68"/>
+      <c r="J50" s="69"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="28"/>
@@ -1822,8 +1830,8 @@
       <c r="F51" s="36"/>
       <c r="G51" s="21"/>
       <c r="H51" s="41"/>
-      <c r="I51" s="48"/>
-      <c r="J51" s="49"/>
+      <c r="I51" s="68"/>
+      <c r="J51" s="69"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="28"/>
@@ -1834,8 +1842,8 @@
       <c r="F52" s="36"/>
       <c r="G52" s="21"/>
       <c r="H52" s="26"/>
-      <c r="I52" s="52"/>
-      <c r="J52" s="53"/>
+      <c r="I52" s="70"/>
+      <c r="J52" s="71"/>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="28"/>
@@ -1846,8 +1854,8 @@
       <c r="F53" s="36"/>
       <c r="G53" s="21"/>
       <c r="H53" s="26"/>
-      <c r="I53" s="52"/>
-      <c r="J53" s="53"/>
+      <c r="I53" s="70"/>
+      <c r="J53" s="71"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="20"/>
@@ -1858,8 +1866,8 @@
       <c r="F54" s="26"/>
       <c r="G54" s="20"/>
       <c r="H54" s="26"/>
-      <c r="I54" s="48"/>
-      <c r="J54" s="49"/>
+      <c r="I54" s="68"/>
+      <c r="J54" s="69"/>
     </row>
     <row r="55" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="20"/>
@@ -1870,8 +1878,8 @@
       <c r="F55" s="26"/>
       <c r="G55" s="20"/>
       <c r="H55" s="26"/>
-      <c r="I55" s="48"/>
-      <c r="J55" s="49"/>
+      <c r="I55" s="68"/>
+      <c r="J55" s="69"/>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="20"/>
@@ -1882,8 +1890,8 @@
       <c r="F56" s="26"/>
       <c r="G56" s="20"/>
       <c r="H56" s="26"/>
-      <c r="I56" s="48"/>
-      <c r="J56" s="49"/>
+      <c r="I56" s="68"/>
+      <c r="J56" s="69"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="20"/>
@@ -1894,8 +1902,8 @@
       <c r="F57" s="26"/>
       <c r="G57" s="20"/>
       <c r="H57" s="26"/>
-      <c r="I57" s="48"/>
-      <c r="J57" s="49"/>
+      <c r="I57" s="68"/>
+      <c r="J57" s="69"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" s="20"/>
@@ -1906,8 +1914,8 @@
       <c r="F58" s="26"/>
       <c r="G58" s="20"/>
       <c r="H58" s="26"/>
-      <c r="I58" s="48"/>
-      <c r="J58" s="49"/>
+      <c r="I58" s="68"/>
+      <c r="J58" s="69"/>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="20"/>
@@ -1917,8 +1925,8 @@
       <c r="F59" s="26"/>
       <c r="G59" s="20"/>
       <c r="H59" s="26"/>
-      <c r="I59" s="48"/>
-      <c r="J59" s="49"/>
+      <c r="I59" s="68"/>
+      <c r="J59" s="69"/>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="20"/>
@@ -1929,8 +1937,8 @@
       <c r="F60" s="26"/>
       <c r="G60" s="20"/>
       <c r="H60" s="26"/>
-      <c r="I60" s="48"/>
-      <c r="J60" s="49"/>
+      <c r="I60" s="68"/>
+      <c r="J60" s="69"/>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="20"/>
@@ -1941,8 +1949,8 @@
       <c r="F61" s="26"/>
       <c r="G61" s="20"/>
       <c r="H61" s="26"/>
-      <c r="I61" s="48"/>
-      <c r="J61" s="49"/>
+      <c r="I61" s="68"/>
+      <c r="J61" s="69"/>
     </row>
     <row r="62" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A62" s="37"/>
@@ -1953,8 +1961,8 @@
       <c r="F62" s="40"/>
       <c r="G62" s="37"/>
       <c r="H62" s="40"/>
-      <c r="I62" s="50"/>
-      <c r="J62" s="51"/>
+      <c r="I62" s="72"/>
+      <c r="J62" s="73"/>
     </row>
     <row r="63" spans="1:10" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1"/>
@@ -2096,19 +2104,36 @@
     </row>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:J6"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="F9:J11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="A5:J5"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:J7"/>
+    <mergeCell ref="I58:J58"/>
+    <mergeCell ref="I59:J59"/>
+    <mergeCell ref="I60:J60"/>
+    <mergeCell ref="I61:J61"/>
+    <mergeCell ref="I62:J62"/>
+    <mergeCell ref="I53:J53"/>
+    <mergeCell ref="I54:J54"/>
+    <mergeCell ref="I55:J55"/>
+    <mergeCell ref="I56:J56"/>
+    <mergeCell ref="I57:J57"/>
+    <mergeCell ref="I48:J48"/>
+    <mergeCell ref="I49:J49"/>
+    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="I51:J51"/>
+    <mergeCell ref="I52:J52"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="I45:J45"/>
+    <mergeCell ref="I46:J46"/>
+    <mergeCell ref="I47:J47"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="I41:J41"/>
+    <mergeCell ref="I42:J42"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="I37:J37"/>
     <mergeCell ref="I29:J29"/>
     <mergeCell ref="I30:J30"/>
     <mergeCell ref="I31:J31"/>
@@ -2122,36 +2147,19 @@
     <mergeCell ref="I28:J28"/>
     <mergeCell ref="I22:J22"/>
     <mergeCell ref="I23:J23"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="I35:J35"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="I37:J37"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="I39:J39"/>
-    <mergeCell ref="I40:J40"/>
-    <mergeCell ref="I41:J41"/>
-    <mergeCell ref="I42:J42"/>
-    <mergeCell ref="I43:J43"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="I45:J45"/>
-    <mergeCell ref="I46:J46"/>
-    <mergeCell ref="I47:J47"/>
-    <mergeCell ref="I48:J48"/>
-    <mergeCell ref="I49:J49"/>
-    <mergeCell ref="I50:J50"/>
-    <mergeCell ref="I51:J51"/>
-    <mergeCell ref="I52:J52"/>
-    <mergeCell ref="I53:J53"/>
-    <mergeCell ref="I54:J54"/>
-    <mergeCell ref="I55:J55"/>
-    <mergeCell ref="I56:J56"/>
-    <mergeCell ref="I57:J57"/>
-    <mergeCell ref="I58:J58"/>
-    <mergeCell ref="I59:J59"/>
-    <mergeCell ref="I60:J60"/>
-    <mergeCell ref="I61:J61"/>
-    <mergeCell ref="I62:J62"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:J7"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:J6"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="F9:J11"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions gridLines="1" gridLinesSet="0"/>

</xml_diff>